<commit_message>
Luq/add logout script (#221)
* [ci skip]

* [ci skip]
</commit_message>
<xml_diff>
--- a/webvitals/resources/testdata.xlsx
+++ b/webvitals/resources/testdata.xlsx
@@ -427,13 +427,13 @@
         <v>Desktop</v>
       </c>
       <c r="C2">
-        <v>4535.699999999233</v>
+        <v>4869.300000000134</v>
       </c>
       <c r="D2">
         <v>0.000723548</v>
       </c>
       <c r="E2">
-        <v>16628.5</v>
+        <v>16195</v>
       </c>
     </row>
     <row r="3">
@@ -444,13 +444,13 @@
         <v>iPhoneX</v>
       </c>
       <c r="C3">
-        <v>4502.94999999995</v>
+        <v>4768.7999999999</v>
       </c>
       <c r="D3">
-        <v>0.00041082339999999997</v>
+        <v>0.000723548</v>
       </c>
       <c r="E3">
-        <v>17644.5</v>
+        <v>18477</v>
       </c>
     </row>
     <row r="4">
@@ -461,13 +461,13 @@
         <v>Desktop</v>
       </c>
       <c r="C4">
-        <v>3853.05000000005</v>
+        <v>4735.900000000067</v>
       </c>
       <c r="D4">
-        <v>0.0022867158</v>
+        <v>0.0030348684</v>
       </c>
       <c r="E4">
-        <v>16414.666666666668</v>
+        <v>18292.333333333332</v>
       </c>
     </row>
     <row r="5">
@@ -478,13 +478,13 @@
         <v>iPhoneX</v>
       </c>
       <c r="C5">
-        <v>4502.6999999992495</v>
+        <v>4735.300000000033</v>
       </c>
       <c r="D5">
-        <v>0.0030303434</v>
+        <v>0.0030348684</v>
       </c>
       <c r="E5">
-        <v>16359.333333333334</v>
+        <v>18277.333333333332</v>
       </c>
     </row>
     <row r="6">
@@ -495,13 +495,13 @@
         <v>Desktop</v>
       </c>
       <c r="C6">
-        <v>4003</v>
+        <v>4636.566666666734</v>
       </c>
       <c r="D6">
-        <v>0.0030379324000000003</v>
+        <v>0.0022970415</v>
       </c>
       <c r="E6">
-        <v>16402.333333333332</v>
+        <v>19603.333333333332</v>
       </c>
     </row>
     <row r="7">
@@ -512,13 +512,13 @@
         <v>iPhoneX</v>
       </c>
       <c r="C7">
-        <v>3853.50000000045</v>
+        <v>4635.366666666533</v>
       </c>
       <c r="D7">
-        <v>0.0022358506000000004</v>
+        <v>0.0022970415000000003</v>
       </c>
       <c r="E7">
-        <v>16439.5</v>
+        <v>19502.333333333332</v>
       </c>
     </row>
     <row r="8">
@@ -529,13 +529,13 @@
         <v>Desktop</v>
       </c>
       <c r="C8">
-        <v>4502.433333334833</v>
+        <v>4535.5333333332665</v>
       </c>
       <c r="D8">
         <v>0.0015430881999999998</v>
       </c>
       <c r="E8">
-        <v>13387.333333333334</v>
+        <v>15587.666666666666</v>
       </c>
     </row>
     <row r="9">
@@ -546,13 +546,13 @@
         <v>iPhoneX</v>
       </c>
       <c r="C9">
-        <v>4103.049999994</v>
+        <v>4602.7666666666</v>
       </c>
       <c r="D9">
         <v>0.0015430881999999998</v>
       </c>
       <c r="E9">
-        <v>13280.666666666666</v>
+        <v>15527.666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>